<commit_message>
scale data push and pull
</commit_message>
<xml_diff>
--- a/data-raw/data-tidy/tech-yearbook/part08-output/03-teckmarket-pull/funds-2000.xlsx
+++ b/data-raw/data-tidy/tech-yearbook/part08-output/03-teckmarket-pull/funds-2000.xlsx
@@ -500,7 +500,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>6.6604</v>
+        <v>66604</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -520,7 +520,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="n">
-        <v>103.1906</v>
+        <v>1031906</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -540,7 +540,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="n">
-        <v>19.3767</v>
+        <v>193767</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -560,7 +560,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="n">
-        <v>5.4557</v>
+        <v>54557</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -580,7 +580,7 @@
         <v>8</v>
       </c>
       <c r="D6" t="n">
-        <v>66.9783</v>
+        <v>669783</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -600,7 +600,7 @@
         <v>8</v>
       </c>
       <c r="D7" t="n">
-        <v>3.8736</v>
+        <v>38736</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -620,7 +620,7 @@
         <v>8</v>
       </c>
       <c r="D8" t="n">
-        <v>1.6522</v>
+        <v>16522</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -640,7 +640,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>1.4795</v>
+        <v>14795</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -660,7 +660,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="n">
-        <v>16.395</v>
+        <v>163950</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -680,7 +680,7 @@
         <v>8</v>
       </c>
       <c r="D11" t="n">
-        <v>19.0434</v>
+        <v>190434</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -700,7 +700,7 @@
         <v>8</v>
       </c>
       <c r="D12" t="n">
-        <v>15.5168</v>
+        <v>155168</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
@@ -720,7 +720,7 @@
         <v>8</v>
       </c>
       <c r="D13" t="n">
-        <v>19.0942</v>
+        <v>190942</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
@@ -740,7 +740,7 @@
         <v>8</v>
       </c>
       <c r="D14" t="n">
-        <v>22.74</v>
+        <v>227400</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
@@ -760,7 +760,7 @@
         <v>8</v>
       </c>
       <c r="D15" t="n">
-        <v>7.8926</v>
+        <v>78926</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
@@ -780,7 +780,7 @@
         <v>8</v>
       </c>
       <c r="D16" t="n">
-        <v>41.1821</v>
+        <v>411821</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
@@ -800,7 +800,7 @@
         <v>8</v>
       </c>
       <c r="D17" t="n">
-        <v>6.6104</v>
+        <v>66104</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
@@ -820,7 +820,7 @@
         <v>8</v>
       </c>
       <c r="D18" t="n">
-        <v>32.6885</v>
+        <v>326885</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
@@ -840,7 +840,7 @@
         <v>8</v>
       </c>
       <c r="D19" t="n">
-        <v>7.96</v>
+        <v>79600</v>
       </c>
       <c r="E19" t="s">
         <v>9</v>
@@ -860,7 +860,7 @@
         <v>8</v>
       </c>
       <c r="D20" t="n">
-        <v>0.9752</v>
+        <v>9752</v>
       </c>
       <c r="E20" t="s">
         <v>9</v>
@@ -880,7 +880,7 @@
         <v>8</v>
       </c>
       <c r="D21" t="n">
-        <v>0.7628</v>
+        <v>7628</v>
       </c>
       <c r="E21" t="s">
         <v>9</v>
@@ -900,7 +900,7 @@
         <v>8</v>
       </c>
       <c r="D22" t="n">
-        <v>650.7519</v>
+        <v>6507519</v>
       </c>
       <c r="E22" t="s">
         <v>9</v>
@@ -920,7 +920,7 @@
         <v>8</v>
       </c>
       <c r="D23" t="n">
-        <v>34.561</v>
+        <v>345610</v>
       </c>
       <c r="E23" t="s">
         <v>9</v>
@@ -940,7 +940,7 @@
         <v>8</v>
       </c>
       <c r="D24" t="n">
-        <v>4.935</v>
+        <v>49350</v>
       </c>
       <c r="E24" t="s">
         <v>9</v>
@@ -960,7 +960,7 @@
         <v>8</v>
       </c>
       <c r="D25" t="n">
-        <v>8.4188</v>
+        <v>84188</v>
       </c>
       <c r="E25" t="s">
         <v>9</v>
@@ -980,7 +980,7 @@
         <v>8</v>
       </c>
       <c r="D26" t="n">
-        <v>63.3736</v>
+        <v>633736</v>
       </c>
       <c r="E26" t="s">
         <v>9</v>
@@ -1000,7 +1000,7 @@
         <v>8</v>
       </c>
       <c r="D27" t="n">
-        <v>12.859</v>
+        <v>128590</v>
       </c>
       <c r="E27" t="s">
         <v>9</v>
@@ -1020,7 +1020,7 @@
         <v>8</v>
       </c>
       <c r="D28" t="n">
-        <v>23.1158</v>
+        <v>231158</v>
       </c>
       <c r="E28" t="s">
         <v>9</v>
@@ -1040,7 +1040,7 @@
         <v>8</v>
       </c>
       <c r="D29" t="n">
-        <v>0.2994</v>
+        <v>2994</v>
       </c>
       <c r="E29" t="s">
         <v>9</v>
@@ -1060,7 +1060,7 @@
         <v>8</v>
       </c>
       <c r="D30" t="n">
-        <v>8.2847</v>
+        <v>82847</v>
       </c>
       <c r="E30" t="s">
         <v>9</v>
@@ -1080,7 +1080,7 @@
         <v>8</v>
       </c>
       <c r="D31" t="n">
-        <v>22.8497</v>
+        <v>228497</v>
       </c>
       <c r="E31" t="s">
         <v>9</v>
@@ -1100,7 +1100,7 @@
         <v>8</v>
       </c>
       <c r="D32" t="n">
-        <v>30.3584</v>
+        <v>303584</v>
       </c>
       <c r="E32" t="s">
         <v>9</v>
@@ -1120,7 +1120,7 @@
         <v>8</v>
       </c>
       <c r="D33" t="n">
-        <v>16.45</v>
+        <v>164500</v>
       </c>
       <c r="E33" t="s">
         <v>9</v>

</xml_diff>